<commit_message>
thêm table vào template của excel
</commit_message>
<xml_diff>
--- a/UserServices.Api/wwwroot/Template/AddUsers.xlsx
+++ b/UserServices.Api/wwwroot/Template/AddUsers.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Asp.net project\ApecMovie\UserServices.Api\wwwroot\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91BE9599-39A0-4837-9E24-E3C1E7AE4231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D637C29A-1C5E-40F4-A4C0-0B4F99AD365A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{08BF945F-0F71-48BC-8AEA-0622C5B59D30}"/>
   </bookViews>
@@ -86,6 +86,18 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E6BEFA9F-BDF8-4052-A5D9-01730ADE57CC}" name="Table1" displayName="Table1" ref="A1:C24" totalsRowShown="0">
+  <autoFilter ref="A1:C24" xr:uid="{E6BEFA9F-BDF8-4052-A5D9-01730ADE57CC}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{1EB1A803-A345-4817-9B0E-765F18F1493B}" name="Tên"/>
+    <tableColumn id="2" xr3:uid="{13B622F8-1665-444C-B96A-AD73AAE7BF01}" name="Email"/>
+    <tableColumn id="3" xr3:uid="{4171D46A-576B-4856-9772-BD18745ACFFD}" name="Mật khẩu"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -388,13 +400,14 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="20.21875" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="2" max="2" width="33.109375" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -412,5 +425,8 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>